<commit_message>
Updated the board to fix alot of stuff
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Desktop\Stuff\Work_Files\Makerspace_THT_Workshop_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24130F-24FC-4067-8B6C-F94DF7900261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF551A3-4C80-4883-906B-567C874777F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,12 +116,6 @@
     <t>Battery Holder</t>
   </si>
   <si>
-    <t>36-3001-ND BATT RETAINER COIN 12MM PC PIN</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/3001/227442</t>
-  </si>
-  <si>
     <t>OP Amp IC</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">Total Part Count = </t>
+  </si>
+  <si>
+    <t>BATT RETAINER COIN 20MM PC PIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/mpd-memory-protection-devices/BK-913/2329371</t>
   </si>
 </sst>
 </file>
@@ -308,9 +308,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -330,7 +327,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,7 +617,7 @@
   <dimension ref="A1:AA42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -632,35 +632,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -681,37 +681,37 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="10">
         <f>SUM(E3:E123)</f>
-        <v>6.51</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="15">
+        <v>6.59</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" s="14">
         <f>SUM(C3:C17)</f>
         <v>22</v>
       </c>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
     </row>
     <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -730,7 +730,7 @@
         <f>(C3*D3)</f>
         <v>1.46</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -754,7 +754,7 @@
         <f>(C4*D4)</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -768,14 +768,14 @@
       <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.18</v>
       </c>
       <c r="E5" s="6">
         <f>(C5*D5)</f>
         <v>0.36</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -783,7 +783,7 @@
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="5">
@@ -796,7 +796,7 @@
         <f>(C6*D6)</f>
         <v>0.31</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -810,14 +810,14 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>0.71</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" ref="E7:E29" si="0">(C7*D7)</f>
+        <f t="shared" ref="E7:E17" si="0">(C7*D7)</f>
         <v>0.71</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -825,21 +825,21 @@
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>26</v>
+      <c r="B8" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="D8" s="6">
-        <v>0.47</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>27</v>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>19</v>
@@ -847,10 +847,10 @@
     </row>
     <row r="9" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -862,16 +862,16 @@
         <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>30</v>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -883,16 +883,16 @@
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>33</v>
+      <c r="F10" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5">
         <v>5</v>
@@ -904,16 +904,16 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>38</v>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -925,16 +925,16 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>37</v>
+      <c r="F12" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5">
         <v>2</v>
@@ -946,16 +946,16 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>40</v>
+      <c r="F13" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -967,16 +967,16 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>45</v>
+      <c r="F14" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -988,16 +988,16 @@
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>48</v>
+      <c r="F15" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1009,16 +1009,16 @@
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>51</v>
+      <c r="F16" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1030,8 +1030,8 @@
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>54</v>
+      <c r="F17" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1131,16 +1131,16 @@
     <hyperlink ref="F5" r:id="rId3" xr:uid="{77130A66-959F-4FBB-9096-D5739FA7DC09}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{51EE6580-D781-4821-BF04-BECDB0756FF2}"/>
     <hyperlink ref="F7" r:id="rId5" xr:uid="{13DBC5BB-CC3E-454E-B7B1-5A7F92EBAAC0}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{C98A2E1C-591F-4A19-8084-028685FBC569}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{E839B0C0-995B-4B90-A675-312C1BFC0788}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{B283E8A8-C87A-44CF-932C-3AC83B12C324}"/>
-    <hyperlink ref="F12" r:id="rId9" xr:uid="{8940FE0F-783F-4C53-A6DB-5E02FDC0E773}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{2101284D-1DF3-420D-8F28-F47248FFFF84}"/>
-    <hyperlink ref="F13" r:id="rId11" xr:uid="{689488C3-70C2-45CB-97A0-5F3BC351F20D}"/>
-    <hyperlink ref="F14" r:id="rId12" xr:uid="{FDC97249-B278-409F-9206-0D30D8935EF9}"/>
-    <hyperlink ref="F15" r:id="rId13" xr:uid="{0CDE6BCC-858D-4A98-AFDD-8BEE9F87C6C1}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{968BBC9A-9A57-4D01-95C9-DB9F08FE158E}"/>
-    <hyperlink ref="F17" r:id="rId15" xr:uid="{3E6E6E18-C439-4F11-BBE6-2253A1A3B59B}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{E839B0C0-995B-4B90-A675-312C1BFC0788}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{B283E8A8-C87A-44CF-932C-3AC83B12C324}"/>
+    <hyperlink ref="F12" r:id="rId8" xr:uid="{8940FE0F-783F-4C53-A6DB-5E02FDC0E773}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{2101284D-1DF3-420D-8F28-F47248FFFF84}"/>
+    <hyperlink ref="F13" r:id="rId10" xr:uid="{689488C3-70C2-45CB-97A0-5F3BC351F20D}"/>
+    <hyperlink ref="F14" r:id="rId11" xr:uid="{FDC97249-B278-409F-9206-0D30D8935EF9}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{0CDE6BCC-858D-4A98-AFDD-8BEE9F87C6C1}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{968BBC9A-9A57-4D01-95C9-DB9F08FE158E}"/>
+    <hyperlink ref="F17" r:id="rId14" xr:uid="{3E6E6E18-C439-4F11-BBE6-2253A1A3B59B}"/>
+    <hyperlink ref="F8" r:id="rId15" xr:uid="{46B42AD8-DB2A-4CE9-952F-BF3F0EA0BC30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>